<commit_message>
Redoing the Godot setup to better fit Godot design principles
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ce633550331854b/Games by Zoe Locke/Potential_Game/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Potential_Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{2FC1EEC4-F4F4-43A2-BDAA-2AC16A8795A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD055F2F-5A50-4451-B4C7-651352FF358A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2360008A-DAA9-4065-80AA-50DA35D22A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{6C05DBB5-C9D8-4AAA-9053-D7ABFE5B0349}"/>
   </bookViews>
@@ -35,54 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
-  <si>
-    <t>Screen w</t>
-  </si>
-  <si>
-    <t>Screen h</t>
-  </si>
-  <si>
-    <t>hex w</t>
-  </si>
-  <si>
-    <t>hex h</t>
-  </si>
-  <si>
-    <t>hex o w</t>
-  </si>
-  <si>
-    <t>hex o h</t>
-  </si>
-  <si>
-    <t>Screen m w</t>
-  </si>
-  <si>
-    <t>Screen m h</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Hex</t>
   </si>
@@ -207,10 +161,13 @@
     <t>1,3</t>
   </si>
   <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>H</t>
+    <t>MoveX</t>
+  </si>
+  <si>
+    <t>MoveY</t>
+  </si>
+  <si>
+    <t>OffsetX</t>
   </si>
 </sst>
 </file>
@@ -275,24 +232,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3B83381A-1947-4D98-9442-AE71ADF55ED6}" name="Table1" displayName="Table1" ref="A1:H2" totalsRowShown="0">
-  <autoFilter ref="A1:H2" xr:uid="{3B83381A-1947-4D98-9442-AE71ADF55ED6}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{521B1068-30EE-4BED-AA06-E639DD086DE5}" name="Screen w"/>
-    <tableColumn id="2" xr3:uid="{08A4B09C-59FF-4FBC-8788-C449D40D9766}" name="Screen h"/>
-    <tableColumn id="3" xr3:uid="{BC0AB2B8-B9DD-415C-96CE-4A262B199C06}" name="hex w"/>
-    <tableColumn id="4" xr3:uid="{F3D9D966-AFDD-476E-90B8-6CA030ABF282}" name="hex h"/>
-    <tableColumn id="5" xr3:uid="{C1688A5F-3540-461F-B3CB-A15BE380E7EE}" name="Screen m w">
-      <calculatedColumnFormula>A2/2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{51F8982B-B8B9-4DF0-B9A4-10A451571F62}" name="Screen m h">
-      <calculatedColumnFormula>B2/2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{3D091BA7-8F39-4B26-881E-BDB1F7AA24E1}" name="hex o w">
-      <calculatedColumnFormula>C2/2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{AADCD1D5-9B49-46BE-AE49-8685AE630BE1}" name="hex o h">
-      <calculatedColumnFormula>D2/2</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33520724-BB8B-45CD-BF4A-2E89AF01227C}" name="Table1" displayName="Table1" ref="A1:C2" totalsRowShown="0">
+  <autoFilter ref="A1:C2" xr:uid="{33520724-BB8B-45CD-BF4A-2E89AF01227C}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0D9D55B9-C85E-4407-9FB1-BF8760600CE3}" name="MoveX"/>
+    <tableColumn id="2" xr3:uid="{1E40AE66-E0F6-40C9-8B99-84537B82F3F5}" name="MoveY"/>
+    <tableColumn id="3" xr3:uid="{C1219D67-4E9B-479F-87E2-65400723BA56}" name="OffsetX">
+      <calculatedColumnFormula>Table1[[#This Row],[MoveX]]/2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -619,7 +565,7 @@
   <dimension ref="A1:L55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,287 +588,143 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>1920</v>
+        <v>198</v>
       </c>
       <c r="B2">
-        <v>1080</v>
+        <v>170</v>
       </c>
       <c r="C2">
-        <v>198</v>
-      </c>
-      <c r="D2">
-        <v>228</v>
-      </c>
-      <c r="E2">
-        <f>A2/2</f>
-        <v>960</v>
-      </c>
-      <c r="F2">
-        <f>B2/2</f>
-        <v>540</v>
-      </c>
-      <c r="G2">
-        <f>C2/2</f>
+        <f>Table1[[#This Row],[MoveX]]/2</f>
         <v>99</v>
-      </c>
-      <c r="H2">
-        <f>D2/2</f>
-        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>762</v>
-      </c>
-      <c r="C5">
-        <v>150</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>960</v>
-      </c>
-      <c r="C6">
-        <v>150</v>
-      </c>
-      <c r="I6" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" cm="1">
-        <f t="array" ref="J6">Table1[hex w]/4</f>
-        <v>49.5</v>
-      </c>
-      <c r="K6">
-        <f>J6*3</f>
-        <v>148.5</v>
-      </c>
-      <c r="L6" s="1">
-        <f>K6-1</f>
-        <v>147.5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>1158</v>
-      </c>
-      <c r="C7">
-        <v>150</v>
-      </c>
-      <c r="I7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" cm="1">
-        <f t="array" ref="J7">Table1[hex h]/4</f>
-        <v>57</v>
-      </c>
-      <c r="K7">
-        <f>J7*3</f>
-        <v>171</v>
-      </c>
-      <c r="L7" s="1">
-        <f>K7-1</f>
-        <v>170</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="L7" s="1"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>862</v>
-      </c>
-      <c r="C9">
-        <f>$C$7+$L$7</f>
-        <v>320</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" cm="1">
-        <f t="array" ref="B10">B9+Table1[hex w]</f>
-        <v>1060</v>
-      </c>
-      <c r="C10">
-        <f t="shared" ref="C10:C12" si="0">$C$7+$L$7</f>
-        <v>320</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" cm="1">
-        <f t="array" ref="B11">B10+Table1[hex w]</f>
-        <v>1258</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>320</v>
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <f>1920/2</f>
+        <v>960</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" cm="1">
-        <f t="array" ref="B12">B11+Table1[hex w]</f>
-        <v>1456</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>320</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <v>565</v>
-      </c>
-      <c r="C14">
-        <f>C12+L7</f>
-        <v>490</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" cm="1">
-        <f t="array" ref="B15">B14+Table1[hex w]</f>
-        <v>763</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" cm="1">
-        <f t="array" ref="B16">B15+Table1[hex w]</f>
-        <v>961</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" cm="1">
-        <f t="array" ref="B17">B16+Table1[hex w]</f>
-        <v>1159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" cm="1">
-        <f t="array" ref="B18">B17+Table1[hex w]</f>
-        <v>1357</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" cm="1">
-        <f t="array" ref="B20">B14+Table1[hex w]</f>
-        <v>763</v>
-      </c>
-      <c r="C20" cm="1">
-        <f t="array" ref="C20">C14+Table1[hex h]</f>
-        <v>718</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23">
-        <f>664+198</f>
-        <v>862</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="H24">
-        <f>H23+198</f>
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="10:11" x14ac:dyDescent="0.35">
@@ -931,169 +733,169 @@
         <v>2,0</v>
       </c>
       <c r="K37" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J38" t="str">
-        <f t="shared" ref="J38:J55" si="1">_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(K38,": ")," |")</f>
+        <f t="shared" ref="J38:J55" si="0">_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(K38,": ")," |")</f>
         <v>3,0</v>
       </c>
       <c r="K38" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4,0</v>
       </c>
       <c r="K39" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1,1</v>
       </c>
       <c r="K40" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2,1</v>
       </c>
       <c r="K41" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3,1</v>
       </c>
       <c r="K42" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4,1</v>
       </c>
       <c r="K43" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0,2</v>
       </c>
       <c r="K44" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1,2</v>
       </c>
       <c r="K45" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2,2</v>
       </c>
       <c r="K46" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3,2</v>
       </c>
       <c r="K47" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4,2</v>
       </c>
       <c r="K48" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0,3</v>
       </c>
       <c r="K49" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1,3</v>
       </c>
       <c r="K50" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2,3</v>
       </c>
       <c r="K51" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3,3</v>
       </c>
       <c r="K52" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0,4</v>
       </c>
       <c r="K53" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1,4</v>
       </c>
       <c r="K54" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="10:11" x14ac:dyDescent="0.35">
       <c r="J55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2,4</v>
       </c>
       <c r="K55" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>